<commit_message>
Fixes #4 and Fixes #5 . Added gerber 1.4.1 for hotplate with corrected playout and removed 1.4 and fixed Inductor note in the BOM
</commit_message>
<xml_diff>
--- a/Hardware/1 Zone/BOM/BOM_V1.4-Wifi_V1.4-Wifi_2024-02-10.xlsx
+++ b/Hardware/1 Zone/BOM/BOM_V1.4-Wifi_V1.4-Wifi_2024-02-10.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F75797-BF6A-40F6-A4B5-EEE646C75E3E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{311344AA-D472-4179-B871-968191E3ADD1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="76800" windowHeight="17625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="885" uniqueCount="325">
   <si>
     <t>No.</t>
   </si>
@@ -455,12 +455,6 @@
     <t>IND-SMD_L7.3-W7.3_CDRH74</t>
   </si>
   <si>
-    <t>CDRH74-220MT</t>
-  </si>
-  <si>
-    <t>MetalLions(美铼)</t>
-  </si>
-  <si>
     <t>SMD,7.3x7.3mm</t>
   </si>
   <si>
@@ -981,16 +975,39 @@
   </si>
   <si>
     <t>0.1154</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>CDRH74-221MT</t>
+  </si>
+  <si>
+    <t>220uH (CD74R-221)</t>
+  </si>
+  <si>
+    <t>AliExpress</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/1005005453639618.html?spm=a2g0o.productlist.main.7.fc121f071PKJLW&amp;algo_pvid=f9629d7f-965b-4802-a78f-4d249e8c6e80&amp;algo_exp_id=f9629d7f-965b-4802-a78f-4d249e8c6e80-3&amp;pdp_npi=4%40dis%21BGN%214.20%213.99%21%21%2116.56%2115.73%21%402101c5a417171395910791417e39c0%2112000033143312160%21sea%21BG%213156952160%21&amp;curPageLogUid=4Y1aJAra4aBs&amp;utparam-url=scene%3Asearch%7Cquery_from%3A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1013,13 +1030,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1359,8 +1379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G63" sqref="G63"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2424,28 +2444,28 @@
         <v>143</v>
       </c>
       <c r="G23" t="s">
-        <v>146</v>
-      </c>
-      <c r="H23" t="s">
-        <v>147</v>
+        <v>322</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>324</v>
       </c>
       <c r="I23" t="s">
-        <v>31</v>
+        <v>323</v>
       </c>
       <c r="J23" t="s">
-        <v>22</v>
+        <v>320</v>
       </c>
       <c r="K23" t="s">
         <v>27</v>
       </c>
       <c r="L23" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="M23" t="s">
         <v>31</v>
       </c>
       <c r="N23" t="s">
-        <v>146</v>
+        <v>321</v>
       </c>
       <c r="O23" t="s">
         <v>31</v>
@@ -2462,10 +2482,10 @@
         <v>31</v>
       </c>
       <c r="D24" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E24" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F24" t="s">
         <v>31</v>
@@ -2492,7 +2512,7 @@
         <v>31</v>
       </c>
       <c r="N24" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="O24" t="s">
         <v>31</v>
@@ -2506,25 +2526,25 @@
         <v>15</v>
       </c>
       <c r="C25" t="s">
+        <v>150</v>
+      </c>
+      <c r="D25" t="s">
+        <v>151</v>
+      </c>
+      <c r="E25" t="s">
         <v>152</v>
       </c>
-      <c r="D25" t="s">
+      <c r="F25" t="s">
+        <v>31</v>
+      </c>
+      <c r="G25" t="s">
+        <v>150</v>
+      </c>
+      <c r="H25" t="s">
         <v>153</v>
       </c>
-      <c r="E25" t="s">
+      <c r="I25" t="s">
         <v>154</v>
-      </c>
-      <c r="F25" t="s">
-        <v>31</v>
-      </c>
-      <c r="G25" t="s">
-        <v>152</v>
-      </c>
-      <c r="H25" t="s">
-        <v>155</v>
-      </c>
-      <c r="I25" t="s">
-        <v>156</v>
       </c>
       <c r="J25" t="s">
         <v>22</v>
@@ -2539,10 +2559,10 @@
         <v>31</v>
       </c>
       <c r="N25" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="O25" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -2553,25 +2573,25 @@
         <v>15</v>
       </c>
       <c r="C26" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D26" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E26" t="s">
+        <v>152</v>
+      </c>
+      <c r="F26" t="s">
+        <v>31</v>
+      </c>
+      <c r="G26" t="s">
+        <v>157</v>
+      </c>
+      <c r="H26" t="s">
+        <v>153</v>
+      </c>
+      <c r="I26" t="s">
         <v>154</v>
-      </c>
-      <c r="F26" t="s">
-        <v>31</v>
-      </c>
-      <c r="G26" t="s">
-        <v>159</v>
-      </c>
-      <c r="H26" t="s">
-        <v>155</v>
-      </c>
-      <c r="I26" t="s">
-        <v>156</v>
       </c>
       <c r="J26" t="s">
         <v>22</v>
@@ -2586,10 +2606,10 @@
         <v>31</v>
       </c>
       <c r="N26" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="O26" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
@@ -2600,25 +2620,25 @@
         <v>15</v>
       </c>
       <c r="C27" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D27" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E27" t="s">
+        <v>152</v>
+      </c>
+      <c r="F27" t="s">
+        <v>31</v>
+      </c>
+      <c r="G27" t="s">
+        <v>159</v>
+      </c>
+      <c r="H27" t="s">
+        <v>153</v>
+      </c>
+      <c r="I27" t="s">
         <v>154</v>
-      </c>
-      <c r="F27" t="s">
-        <v>31</v>
-      </c>
-      <c r="G27" t="s">
-        <v>161</v>
-      </c>
-      <c r="H27" t="s">
-        <v>155</v>
-      </c>
-      <c r="I27" t="s">
-        <v>156</v>
       </c>
       <c r="J27" t="s">
         <v>22</v>
@@ -2633,10 +2653,10 @@
         <v>31</v>
       </c>
       <c r="N27" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="O27" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
@@ -2647,25 +2667,25 @@
         <v>15</v>
       </c>
       <c r="C28" t="s">
+        <v>161</v>
+      </c>
+      <c r="D28" t="s">
+        <v>162</v>
+      </c>
+      <c r="E28" t="s">
         <v>163</v>
       </c>
-      <c r="D28" t="s">
+      <c r="F28" t="s">
+        <v>31</v>
+      </c>
+      <c r="G28" t="s">
+        <v>161</v>
+      </c>
+      <c r="H28" t="s">
         <v>164</v>
       </c>
-      <c r="E28" t="s">
+      <c r="I28" t="s">
         <v>165</v>
-      </c>
-      <c r="F28" t="s">
-        <v>31</v>
-      </c>
-      <c r="G28" t="s">
-        <v>163</v>
-      </c>
-      <c r="H28" t="s">
-        <v>166</v>
-      </c>
-      <c r="I28" t="s">
-        <v>167</v>
       </c>
       <c r="J28" t="s">
         <v>22</v>
@@ -2674,16 +2694,16 @@
         <v>34</v>
       </c>
       <c r="L28" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="M28" t="s">
         <v>31</v>
       </c>
       <c r="N28" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="O28" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
@@ -2694,25 +2714,25 @@
         <v>15</v>
       </c>
       <c r="C29" t="s">
+        <v>168</v>
+      </c>
+      <c r="D29" t="s">
+        <v>169</v>
+      </c>
+      <c r="E29" t="s">
         <v>170</v>
       </c>
-      <c r="D29" t="s">
+      <c r="F29" t="s">
+        <v>31</v>
+      </c>
+      <c r="G29" t="s">
+        <v>168</v>
+      </c>
+      <c r="H29" t="s">
         <v>171</v>
       </c>
-      <c r="E29" t="s">
+      <c r="I29" t="s">
         <v>172</v>
-      </c>
-      <c r="F29" t="s">
-        <v>31</v>
-      </c>
-      <c r="G29" t="s">
-        <v>170</v>
-      </c>
-      <c r="H29" t="s">
-        <v>173</v>
-      </c>
-      <c r="I29" t="s">
-        <v>174</v>
       </c>
       <c r="J29" t="s">
         <v>22</v>
@@ -2721,16 +2741,16 @@
         <v>53</v>
       </c>
       <c r="L29" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="M29" t="s">
         <v>31</v>
       </c>
       <c r="N29" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="O29" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
@@ -2741,25 +2761,25 @@
         <v>15</v>
       </c>
       <c r="C30" t="s">
+        <v>175</v>
+      </c>
+      <c r="D30" t="s">
+        <v>176</v>
+      </c>
+      <c r="E30" t="s">
         <v>177</v>
       </c>
-      <c r="D30" t="s">
+      <c r="F30" t="s">
+        <v>31</v>
+      </c>
+      <c r="G30" t="s">
+        <v>175</v>
+      </c>
+      <c r="H30" t="s">
         <v>178</v>
       </c>
-      <c r="E30" t="s">
+      <c r="I30" t="s">
         <v>179</v>
-      </c>
-      <c r="F30" t="s">
-        <v>31</v>
-      </c>
-      <c r="G30" t="s">
-        <v>177</v>
-      </c>
-      <c r="H30" t="s">
-        <v>180</v>
-      </c>
-      <c r="I30" t="s">
-        <v>181</v>
       </c>
       <c r="J30" t="s">
         <v>22</v>
@@ -2768,16 +2788,16 @@
         <v>34</v>
       </c>
       <c r="L30" t="s">
+        <v>180</v>
+      </c>
+      <c r="M30" t="s">
+        <v>31</v>
+      </c>
+      <c r="N30" t="s">
+        <v>181</v>
+      </c>
+      <c r="O30" t="s">
         <v>182</v>
-      </c>
-      <c r="M30" t="s">
-        <v>31</v>
-      </c>
-      <c r="N30" t="s">
-        <v>183</v>
-      </c>
-      <c r="O30" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
@@ -2788,25 +2808,25 @@
         <v>15</v>
       </c>
       <c r="C31" t="s">
+        <v>183</v>
+      </c>
+      <c r="D31" t="s">
+        <v>184</v>
+      </c>
+      <c r="E31" t="s">
         <v>185</v>
       </c>
-      <c r="D31" t="s">
+      <c r="F31" t="s">
+        <v>31</v>
+      </c>
+      <c r="G31" t="s">
+        <v>183</v>
+      </c>
+      <c r="H31" t="s">
         <v>186</v>
       </c>
-      <c r="E31" t="s">
+      <c r="I31" t="s">
         <v>187</v>
-      </c>
-      <c r="F31" t="s">
-        <v>31</v>
-      </c>
-      <c r="G31" t="s">
-        <v>185</v>
-      </c>
-      <c r="H31" t="s">
-        <v>188</v>
-      </c>
-      <c r="I31" t="s">
-        <v>189</v>
       </c>
       <c r="J31" t="s">
         <v>22</v>
@@ -2815,16 +2835,16 @@
         <v>34</v>
       </c>
       <c r="L31" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="M31" t="s">
         <v>31</v>
       </c>
       <c r="N31" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="O31" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
@@ -2835,25 +2855,25 @@
         <v>15</v>
       </c>
       <c r="C32" t="s">
+        <v>189</v>
+      </c>
+      <c r="D32" t="s">
+        <v>190</v>
+      </c>
+      <c r="E32" t="s">
         <v>191</v>
       </c>
-      <c r="D32" t="s">
+      <c r="F32" t="s">
+        <v>31</v>
+      </c>
+      <c r="G32" t="s">
+        <v>189</v>
+      </c>
+      <c r="H32" t="s">
         <v>192</v>
       </c>
-      <c r="E32" t="s">
+      <c r="I32" t="s">
         <v>193</v>
-      </c>
-      <c r="F32" t="s">
-        <v>31</v>
-      </c>
-      <c r="G32" t="s">
-        <v>191</v>
-      </c>
-      <c r="H32" t="s">
-        <v>194</v>
-      </c>
-      <c r="I32" t="s">
-        <v>195</v>
       </c>
       <c r="J32" t="s">
         <v>22</v>
@@ -2862,16 +2882,16 @@
         <v>34</v>
       </c>
       <c r="L32" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="M32" t="s">
         <v>31</v>
       </c>
       <c r="N32" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="O32" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
@@ -2882,16 +2902,16 @@
         <v>27</v>
       </c>
       <c r="C33" t="s">
+        <v>196</v>
+      </c>
+      <c r="D33" t="s">
+        <v>197</v>
+      </c>
+      <c r="E33" t="s">
         <v>198</v>
       </c>
-      <c r="D33" t="s">
-        <v>199</v>
-      </c>
-      <c r="E33" t="s">
-        <v>200</v>
-      </c>
       <c r="F33" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G33" t="s">
         <v>31</v>
@@ -2915,7 +2935,7 @@
         <v>31</v>
       </c>
       <c r="N33" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="O33" t="s">
         <v>31</v>
@@ -2929,16 +2949,16 @@
         <v>92</v>
       </c>
       <c r="C34" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D34" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E34" t="s">
+        <v>198</v>
+      </c>
+      <c r="F34" t="s">
         <v>200</v>
-      </c>
-      <c r="F34" t="s">
-        <v>202</v>
       </c>
       <c r="G34" t="s">
         <v>31</v>
@@ -2962,7 +2982,7 @@
         <v>31</v>
       </c>
       <c r="N34" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="O34" t="s">
         <v>31</v>
@@ -2976,16 +2996,16 @@
         <v>65</v>
       </c>
       <c r="C35" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D35" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E35" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F35" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="G35" t="s">
         <v>31</v>
@@ -3009,7 +3029,7 @@
         <v>31</v>
       </c>
       <c r="N35" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="O35" t="s">
         <v>31</v>
@@ -3023,16 +3043,16 @@
         <v>44</v>
       </c>
       <c r="C36" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D36" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E36" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F36" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G36" t="s">
         <v>31</v>
@@ -3056,7 +3076,7 @@
         <v>31</v>
       </c>
       <c r="N36" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="O36" t="s">
         <v>31</v>
@@ -3070,16 +3090,16 @@
         <v>15</v>
       </c>
       <c r="C37" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D37" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E37" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F37" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="G37" t="s">
         <v>31</v>
@@ -3103,7 +3123,7 @@
         <v>31</v>
       </c>
       <c r="N37" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="O37" t="s">
         <v>31</v>
@@ -3117,16 +3137,16 @@
         <v>15</v>
       </c>
       <c r="C38" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D38" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E38" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F38" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="G38" t="s">
         <v>31</v>
@@ -3150,7 +3170,7 @@
         <v>31</v>
       </c>
       <c r="N38" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="O38" t="s">
         <v>31</v>
@@ -3164,16 +3184,16 @@
         <v>15</v>
       </c>
       <c r="C39" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D39" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E39" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F39" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G39" t="s">
         <v>31</v>
@@ -3197,7 +3217,7 @@
         <v>31</v>
       </c>
       <c r="N39" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="O39" t="s">
         <v>31</v>
@@ -3211,22 +3231,22 @@
         <v>53</v>
       </c>
       <c r="C40" t="s">
+        <v>212</v>
+      </c>
+      <c r="D40" t="s">
+        <v>213</v>
+      </c>
+      <c r="E40" t="s">
         <v>214</v>
       </c>
-      <c r="D40" t="s">
+      <c r="F40" t="s">
+        <v>212</v>
+      </c>
+      <c r="G40" t="s">
         <v>215</v>
       </c>
-      <c r="E40" t="s">
+      <c r="H40" t="s">
         <v>216</v>
-      </c>
-      <c r="F40" t="s">
-        <v>214</v>
-      </c>
-      <c r="G40" t="s">
-        <v>217</v>
-      </c>
-      <c r="H40" t="s">
-        <v>218</v>
       </c>
       <c r="I40" t="s">
         <v>31</v>
@@ -3238,13 +3258,13 @@
         <v>34</v>
       </c>
       <c r="L40" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="M40" t="s">
         <v>31</v>
       </c>
       <c r="N40" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="O40" t="s">
         <v>31</v>
@@ -3258,16 +3278,16 @@
         <v>23</v>
       </c>
       <c r="C41" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D41" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E41" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F41" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="G41" t="s">
         <v>31</v>
@@ -3291,7 +3311,7 @@
         <v>31</v>
       </c>
       <c r="N41" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="O41" t="s">
         <v>31</v>
@@ -3305,16 +3325,16 @@
         <v>15</v>
       </c>
       <c r="C42" t="s">
+        <v>220</v>
+      </c>
+      <c r="D42" t="s">
+        <v>221</v>
+      </c>
+      <c r="E42" t="s">
         <v>222</v>
       </c>
-      <c r="D42" t="s">
-        <v>223</v>
-      </c>
-      <c r="E42" t="s">
-        <v>224</v>
-      </c>
       <c r="F42" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G42" t="s">
         <v>31</v>
@@ -3338,7 +3358,7 @@
         <v>31</v>
       </c>
       <c r="N42" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="O42" t="s">
         <v>31</v>
@@ -3352,16 +3372,16 @@
         <v>23</v>
       </c>
       <c r="C43" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D43" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E43" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F43" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G43" t="s">
         <v>31</v>
@@ -3385,7 +3405,7 @@
         <v>31</v>
       </c>
       <c r="N43" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="O43" t="s">
         <v>31</v>
@@ -3399,16 +3419,16 @@
         <v>15</v>
       </c>
       <c r="C44" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D44" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E44" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F44" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G44" t="s">
         <v>31</v>
@@ -3432,7 +3452,7 @@
         <v>31</v>
       </c>
       <c r="N44" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="O44" t="s">
         <v>31</v>
@@ -3446,16 +3466,16 @@
         <v>15</v>
       </c>
       <c r="C45" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D45" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E45" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F45" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G45" t="s">
         <v>31</v>
@@ -3479,7 +3499,7 @@
         <v>31</v>
       </c>
       <c r="N45" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="O45" t="s">
         <v>31</v>
@@ -3493,16 +3513,16 @@
         <v>15</v>
       </c>
       <c r="C46" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D46" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E46" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F46" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G46" t="s">
         <v>31</v>
@@ -3526,7 +3546,7 @@
         <v>31</v>
       </c>
       <c r="N46" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="O46" t="s">
         <v>31</v>
@@ -3540,16 +3560,16 @@
         <v>34</v>
       </c>
       <c r="C47" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D47" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E47" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F47" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G47" t="s">
         <v>31</v>
@@ -3573,7 +3593,7 @@
         <v>31</v>
       </c>
       <c r="N47" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="O47" t="s">
         <v>31</v>
@@ -3587,25 +3607,25 @@
         <v>23</v>
       </c>
       <c r="C48" t="s">
+        <v>231</v>
+      </c>
+      <c r="D48" t="s">
+        <v>232</v>
+      </c>
+      <c r="E48" t="s">
         <v>233</v>
       </c>
-      <c r="D48" t="s">
+      <c r="F48" t="s">
+        <v>31</v>
+      </c>
+      <c r="G48" t="s">
+        <v>231</v>
+      </c>
+      <c r="H48" t="s">
         <v>234</v>
       </c>
-      <c r="E48" t="s">
+      <c r="I48" t="s">
         <v>235</v>
-      </c>
-      <c r="F48" t="s">
-        <v>31</v>
-      </c>
-      <c r="G48" t="s">
-        <v>233</v>
-      </c>
-      <c r="H48" t="s">
-        <v>236</v>
-      </c>
-      <c r="I48" t="s">
-        <v>237</v>
       </c>
       <c r="J48" t="s">
         <v>22</v>
@@ -3614,16 +3634,16 @@
         <v>23</v>
       </c>
       <c r="L48" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="M48" t="s">
         <v>31</v>
       </c>
       <c r="N48" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="O48" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
@@ -3634,25 +3654,25 @@
         <v>15</v>
       </c>
       <c r="C49" t="s">
+        <v>239</v>
+      </c>
+      <c r="D49" t="s">
+        <v>240</v>
+      </c>
+      <c r="E49" t="s">
         <v>241</v>
       </c>
-      <c r="D49" t="s">
+      <c r="F49" t="s">
+        <v>31</v>
+      </c>
+      <c r="G49" t="s">
+        <v>239</v>
+      </c>
+      <c r="H49" t="s">
+        <v>31</v>
+      </c>
+      <c r="I49" t="s">
         <v>242</v>
-      </c>
-      <c r="E49" t="s">
-        <v>243</v>
-      </c>
-      <c r="F49" t="s">
-        <v>31</v>
-      </c>
-      <c r="G49" t="s">
-        <v>241</v>
-      </c>
-      <c r="H49" t="s">
-        <v>31</v>
-      </c>
-      <c r="I49" t="s">
-        <v>244</v>
       </c>
       <c r="J49" t="s">
         <v>22</v>
@@ -3661,13 +3681,13 @@
         <v>34</v>
       </c>
       <c r="L49" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="M49" t="s">
         <v>31</v>
       </c>
       <c r="N49" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="O49" t="s">
         <v>31</v>
@@ -3681,25 +3701,25 @@
         <v>15</v>
       </c>
       <c r="C50" t="s">
+        <v>243</v>
+      </c>
+      <c r="D50" t="s">
+        <v>244</v>
+      </c>
+      <c r="E50" t="s">
         <v>245</v>
       </c>
-      <c r="D50" t="s">
+      <c r="F50" t="s">
+        <v>31</v>
+      </c>
+      <c r="G50" t="s">
+        <v>243</v>
+      </c>
+      <c r="H50" t="s">
         <v>246</v>
       </c>
-      <c r="E50" t="s">
+      <c r="I50" t="s">
         <v>247</v>
-      </c>
-      <c r="F50" t="s">
-        <v>31</v>
-      </c>
-      <c r="G50" t="s">
-        <v>245</v>
-      </c>
-      <c r="H50" t="s">
-        <v>248</v>
-      </c>
-      <c r="I50" t="s">
-        <v>249</v>
       </c>
       <c r="J50" t="s">
         <v>22</v>
@@ -3708,16 +3728,16 @@
         <v>60</v>
       </c>
       <c r="L50" t="s">
+        <v>248</v>
+      </c>
+      <c r="M50" t="s">
+        <v>31</v>
+      </c>
+      <c r="N50" t="s">
+        <v>249</v>
+      </c>
+      <c r="O50" t="s">
         <v>250</v>
-      </c>
-      <c r="M50" t="s">
-        <v>31</v>
-      </c>
-      <c r="N50" t="s">
-        <v>251</v>
-      </c>
-      <c r="O50" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
@@ -3728,25 +3748,25 @@
         <v>15</v>
       </c>
       <c r="C51" t="s">
+        <v>251</v>
+      </c>
+      <c r="D51" t="s">
+        <v>252</v>
+      </c>
+      <c r="E51" t="s">
         <v>253</v>
       </c>
-      <c r="D51" t="s">
+      <c r="F51" t="s">
+        <v>31</v>
+      </c>
+      <c r="G51" t="s">
+        <v>251</v>
+      </c>
+      <c r="H51" t="s">
+        <v>192</v>
+      </c>
+      <c r="I51" t="s">
         <v>254</v>
-      </c>
-      <c r="E51" t="s">
-        <v>255</v>
-      </c>
-      <c r="F51" t="s">
-        <v>31</v>
-      </c>
-      <c r="G51" t="s">
-        <v>253</v>
-      </c>
-      <c r="H51" t="s">
-        <v>194</v>
-      </c>
-      <c r="I51" t="s">
-        <v>256</v>
       </c>
       <c r="J51" t="s">
         <v>22</v>
@@ -3755,16 +3775,16 @@
         <v>23</v>
       </c>
       <c r="L51" t="s">
+        <v>255</v>
+      </c>
+      <c r="M51" t="s">
+        <v>31</v>
+      </c>
+      <c r="N51" t="s">
+        <v>256</v>
+      </c>
+      <c r="O51" t="s">
         <v>257</v>
-      </c>
-      <c r="M51" t="s">
-        <v>31</v>
-      </c>
-      <c r="N51" t="s">
-        <v>258</v>
-      </c>
-      <c r="O51" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
@@ -3775,25 +3795,25 @@
         <v>15</v>
       </c>
       <c r="C52" t="s">
+        <v>258</v>
+      </c>
+      <c r="D52" t="s">
+        <v>259</v>
+      </c>
+      <c r="E52" t="s">
         <v>260</v>
       </c>
-      <c r="D52" t="s">
+      <c r="F52" t="s">
+        <v>31</v>
+      </c>
+      <c r="G52" t="s">
+        <v>258</v>
+      </c>
+      <c r="H52" t="s">
         <v>261</v>
       </c>
-      <c r="E52" t="s">
+      <c r="I52" t="s">
         <v>262</v>
-      </c>
-      <c r="F52" t="s">
-        <v>31</v>
-      </c>
-      <c r="G52" t="s">
-        <v>260</v>
-      </c>
-      <c r="H52" t="s">
-        <v>263</v>
-      </c>
-      <c r="I52" t="s">
-        <v>264</v>
       </c>
       <c r="J52" t="s">
         <v>22</v>
@@ -3808,10 +3828,10 @@
         <v>31</v>
       </c>
       <c r="N52" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="O52" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
@@ -3822,25 +3842,25 @@
         <v>27</v>
       </c>
       <c r="C53" t="s">
+        <v>265</v>
+      </c>
+      <c r="D53" t="s">
+        <v>266</v>
+      </c>
+      <c r="E53" t="s">
         <v>267</v>
       </c>
-      <c r="D53" t="s">
+      <c r="F53" t="s">
+        <v>31</v>
+      </c>
+      <c r="G53" t="s">
+        <v>265</v>
+      </c>
+      <c r="H53" t="s">
         <v>268</v>
       </c>
-      <c r="E53" t="s">
+      <c r="I53" t="s">
         <v>269</v>
-      </c>
-      <c r="F53" t="s">
-        <v>31</v>
-      </c>
-      <c r="G53" t="s">
-        <v>267</v>
-      </c>
-      <c r="H53" t="s">
-        <v>270</v>
-      </c>
-      <c r="I53" t="s">
-        <v>271</v>
       </c>
       <c r="J53" t="s">
         <v>22</v>
@@ -3849,16 +3869,16 @@
         <v>103</v>
       </c>
       <c r="L53" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="M53" t="s">
         <v>31</v>
       </c>
       <c r="N53" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="O53" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
@@ -3869,25 +3889,25 @@
         <v>15</v>
       </c>
       <c r="C54" t="s">
+        <v>272</v>
+      </c>
+      <c r="D54" t="s">
+        <v>273</v>
+      </c>
+      <c r="E54" t="s">
         <v>274</v>
       </c>
-      <c r="D54" t="s">
+      <c r="F54" t="s">
+        <v>31</v>
+      </c>
+      <c r="G54" t="s">
+        <v>272</v>
+      </c>
+      <c r="H54" t="s">
         <v>275</v>
       </c>
-      <c r="E54" t="s">
+      <c r="I54" t="s">
         <v>276</v>
-      </c>
-      <c r="F54" t="s">
-        <v>31</v>
-      </c>
-      <c r="G54" t="s">
-        <v>274</v>
-      </c>
-      <c r="H54" t="s">
-        <v>277</v>
-      </c>
-      <c r="I54" t="s">
-        <v>278</v>
       </c>
       <c r="J54" t="s">
         <v>22</v>
@@ -3896,13 +3916,13 @@
         <v>23</v>
       </c>
       <c r="L54" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="M54" t="s">
         <v>31</v>
       </c>
       <c r="N54" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="O54" t="s">
         <v>31</v>
@@ -3916,25 +3936,25 @@
         <v>15</v>
       </c>
       <c r="C55" t="s">
+        <v>279</v>
+      </c>
+      <c r="D55" t="s">
+        <v>280</v>
+      </c>
+      <c r="E55" t="s">
         <v>281</v>
       </c>
-      <c r="D55" t="s">
+      <c r="F55" t="s">
+        <v>31</v>
+      </c>
+      <c r="G55" t="s">
+        <v>279</v>
+      </c>
+      <c r="H55" t="s">
         <v>282</v>
       </c>
-      <c r="E55" t="s">
+      <c r="I55" t="s">
         <v>283</v>
-      </c>
-      <c r="F55" t="s">
-        <v>31</v>
-      </c>
-      <c r="G55" t="s">
-        <v>281</v>
-      </c>
-      <c r="H55" t="s">
-        <v>284</v>
-      </c>
-      <c r="I55" t="s">
-        <v>285</v>
       </c>
       <c r="J55" t="s">
         <v>22</v>
@@ -3943,13 +3963,13 @@
         <v>60</v>
       </c>
       <c r="L55" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="M55" t="s">
         <v>31</v>
       </c>
       <c r="N55" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="O55" t="s">
         <v>31</v>
@@ -3963,25 +3983,25 @@
         <v>15</v>
       </c>
       <c r="C56" t="s">
+        <v>285</v>
+      </c>
+      <c r="D56" t="s">
+        <v>286</v>
+      </c>
+      <c r="E56" t="s">
         <v>287</v>
       </c>
-      <c r="D56" t="s">
+      <c r="F56" t="s">
+        <v>31</v>
+      </c>
+      <c r="G56" t="s">
+        <v>285</v>
+      </c>
+      <c r="H56" t="s">
         <v>288</v>
       </c>
-      <c r="E56" t="s">
+      <c r="I56" t="s">
         <v>289</v>
-      </c>
-      <c r="F56" t="s">
-        <v>31</v>
-      </c>
-      <c r="G56" t="s">
-        <v>287</v>
-      </c>
-      <c r="H56" t="s">
-        <v>290</v>
-      </c>
-      <c r="I56" t="s">
-        <v>291</v>
       </c>
       <c r="J56" t="s">
         <v>22</v>
@@ -3990,16 +4010,16 @@
         <v>34</v>
       </c>
       <c r="L56" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="M56" t="s">
         <v>31</v>
       </c>
       <c r="N56" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="O56" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
@@ -4010,43 +4030,43 @@
         <v>15</v>
       </c>
       <c r="C57" t="s">
+        <v>291</v>
+      </c>
+      <c r="D57" t="s">
+        <v>292</v>
+      </c>
+      <c r="E57" t="s">
         <v>293</v>
       </c>
-      <c r="D57" t="s">
+      <c r="F57" t="s">
+        <v>31</v>
+      </c>
+      <c r="G57" t="s">
+        <v>291</v>
+      </c>
+      <c r="H57" t="s">
         <v>294</v>
       </c>
-      <c r="E57" t="s">
+      <c r="I57" t="s">
         <v>295</v>
-      </c>
-      <c r="F57" t="s">
-        <v>31</v>
-      </c>
-      <c r="G57" t="s">
-        <v>293</v>
-      </c>
-      <c r="H57" t="s">
-        <v>296</v>
-      </c>
-      <c r="I57" t="s">
-        <v>297</v>
       </c>
       <c r="J57" t="s">
         <v>22</v>
       </c>
       <c r="K57" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="L57" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="M57" t="s">
         <v>31</v>
       </c>
       <c r="N57" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="O57" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
@@ -4057,25 +4077,25 @@
         <v>15</v>
       </c>
       <c r="C58" t="s">
+        <v>298</v>
+      </c>
+      <c r="D58" t="s">
+        <v>299</v>
+      </c>
+      <c r="E58" t="s">
         <v>300</v>
       </c>
-      <c r="D58" t="s">
+      <c r="F58" t="s">
+        <v>31</v>
+      </c>
+      <c r="G58" t="s">
+        <v>298</v>
+      </c>
+      <c r="H58" t="s">
         <v>301</v>
       </c>
-      <c r="E58" t="s">
+      <c r="I58" t="s">
         <v>302</v>
-      </c>
-      <c r="F58" t="s">
-        <v>31</v>
-      </c>
-      <c r="G58" t="s">
-        <v>300</v>
-      </c>
-      <c r="H58" t="s">
-        <v>303</v>
-      </c>
-      <c r="I58" t="s">
-        <v>304</v>
       </c>
       <c r="J58" t="s">
         <v>22</v>
@@ -4084,13 +4104,13 @@
         <v>60</v>
       </c>
       <c r="L58" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="M58" t="s">
         <v>31</v>
       </c>
       <c r="N58" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="O58" t="s">
         <v>31</v>
@@ -4104,25 +4124,25 @@
         <v>27</v>
       </c>
       <c r="C59" t="s">
+        <v>303</v>
+      </c>
+      <c r="D59" t="s">
+        <v>304</v>
+      </c>
+      <c r="E59" t="s">
         <v>305</v>
       </c>
-      <c r="D59" t="s">
+      <c r="F59" t="s">
+        <v>31</v>
+      </c>
+      <c r="G59" t="s">
+        <v>303</v>
+      </c>
+      <c r="H59" t="s">
         <v>306</v>
       </c>
-      <c r="E59" t="s">
+      <c r="I59" t="s">
         <v>307</v>
-      </c>
-      <c r="F59" t="s">
-        <v>31</v>
-      </c>
-      <c r="G59" t="s">
-        <v>305</v>
-      </c>
-      <c r="H59" t="s">
-        <v>308</v>
-      </c>
-      <c r="I59" t="s">
-        <v>309</v>
       </c>
       <c r="J59" t="s">
         <v>22</v>
@@ -4137,10 +4157,10 @@
         <v>31</v>
       </c>
       <c r="N59" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="O59" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
@@ -4151,25 +4171,25 @@
         <v>27</v>
       </c>
       <c r="C60" t="s">
+        <v>309</v>
+      </c>
+      <c r="D60" t="s">
+        <v>310</v>
+      </c>
+      <c r="E60" t="s">
         <v>311</v>
       </c>
-      <c r="D60" t="s">
+      <c r="F60" t="s">
+        <v>31</v>
+      </c>
+      <c r="G60" t="s">
+        <v>309</v>
+      </c>
+      <c r="H60" t="s">
         <v>312</v>
       </c>
-      <c r="E60" t="s">
+      <c r="I60" t="s">
         <v>313</v>
-      </c>
-      <c r="F60" t="s">
-        <v>31</v>
-      </c>
-      <c r="G60" t="s">
-        <v>311</v>
-      </c>
-      <c r="H60" t="s">
-        <v>314</v>
-      </c>
-      <c r="I60" t="s">
-        <v>315</v>
       </c>
       <c r="J60" t="s">
         <v>22</v>
@@ -4178,16 +4198,16 @@
         <v>76</v>
       </c>
       <c r="L60" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="M60" t="s">
         <v>31</v>
       </c>
       <c r="N60" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="O60" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
@@ -4198,25 +4218,25 @@
         <v>15</v>
       </c>
       <c r="C61" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D61" t="s">
         <v>123</v>
       </c>
       <c r="E61" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F61" t="s">
         <v>31</v>
       </c>
       <c r="G61" t="s">
+        <v>316</v>
+      </c>
+      <c r="H61" t="s">
+        <v>312</v>
+      </c>
+      <c r="I61" t="s">
         <v>318</v>
-      </c>
-      <c r="H61" t="s">
-        <v>314</v>
-      </c>
-      <c r="I61" t="s">
-        <v>320</v>
       </c>
       <c r="J61" t="s">
         <v>22</v>
@@ -4225,19 +4245,22 @@
         <v>60</v>
       </c>
       <c r="L61" t="s">
+        <v>314</v>
+      </c>
+      <c r="M61" t="s">
+        <v>31</v>
+      </c>
+      <c r="N61" t="s">
         <v>316</v>
       </c>
-      <c r="M61" t="s">
-        <v>31</v>
-      </c>
-      <c r="N61" t="s">
-        <v>318</v>
-      </c>
       <c r="O61" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H23" r:id="rId1" display="https://www.aliexpress.com/item/1005005453639618.html?spm=a2g0o.productlist.main.7.fc121f071PKJLW&amp;algo_pvid=f9629d7f-965b-4802-a78f-4d249e8c6e80&amp;algo_exp_id=f9629d7f-965b-4802-a78f-4d249e8c6e80-3&amp;pdp_npi=4%40dis%21BGN%214.20%213.99%21%21%2116.56%2115.73%21%402101c5a417171395910791417e39c0%2112000033143312160%21sea%21BG%213156952160%21&amp;curPageLogUid=4Y1aJAra4aBs&amp;utparam-url=scene%3Asearch%7Cquery_from%3A" xr:uid="{27667E32-5828-4878-B274-3BD0D9B7DABE}"/>
+  </hyperlinks>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>

</xml_diff>